<commit_message>
Aman sir suggestions changed
1. Export Custom Selected list
</commit_message>
<xml_diff>
--- a/python_spreadsheet.xlsx
+++ b/python_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\susan\PycharmProjects\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14FBA9B5-D71B-475E-9C9C-E1DB5D8BD230}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A92BAF0-2882-41B8-A2A4-D1D40899CE38}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Subj. Name</t>
   </si>
   <si>
-    <t>PUL</t>
-  </si>
-  <si>
-    <t>Permanent</t>
-  </si>
-  <si>
     <t>Subj. code</t>
   </si>
   <si>
@@ -78,67 +72,7 @@
     <t>Department: Dept. of Electronics and Computer Engineering</t>
   </si>
   <si>
-    <t>Prof. Dr. Subarna Shakya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ph.D. </t>
-  </si>
-  <si>
-    <t>Dr. Sanjeeb Prasad Panday</t>
-  </si>
-  <si>
-    <t>sanjeeb@ioe.edu.np</t>
-  </si>
-  <si>
-    <t>drss@ioe.edu.np</t>
-  </si>
-  <si>
-    <t>15+</t>
-  </si>
-  <si>
-    <t>10+</t>
-  </si>
-  <si>
-    <t>Cloud Computing</t>
-  </si>
-  <si>
-    <t>I/II</t>
-  </si>
-  <si>
-    <t>Image Processing</t>
-  </si>
-  <si>
-    <t>Dr. Basanta Joshi</t>
-  </si>
-  <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>Big Data Applications and Analytics</t>
-  </si>
-  <si>
-    <t>Information Security and Audit</t>
-  </si>
-  <si>
-    <t>Deepen Chapagain</t>
-  </si>
-  <si>
-    <t>4+</t>
-  </si>
-  <si>
-    <t>2+</t>
-  </si>
-  <si>
-    <t>Msc</t>
-  </si>
-  <si>
     <t>24 Poush 2074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">basanta@ioe.edu.np </t>
-  </si>
-  <si>
-    <t xml:space="preserve">deepen@ioe.edu.np </t>
   </si>
   <si>
     <t>Effective Exp. On this subj. till the date)</t>
@@ -617,7 +551,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="M7" sqref="A4:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -640,7 +574,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -648,15 +582,15 @@
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="L1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -664,7 +598,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
@@ -672,184 +606,104 @@
     </row>
     <row r="3" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2">
-        <v>9851212305</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="I4" s="2"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="8">
-        <v>9851190040</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2">
-        <v>9851032303</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I6" s="2"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2">
-        <v>9840052621</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -1172,14 +1026,8 @@
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="D2:I2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="J7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="J6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="J4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-  </hyperlinks>
   <pageMargins left="0.17" right="0.17" top="0.61" bottom="0.44" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId5"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>